<commit_message>
Started with normal distribution
</commit_message>
<xml_diff>
--- a/xlsx/stats.xlsx
+++ b/xlsx/stats.xlsx
@@ -471,7 +471,7 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>cdf</t>
+          <t>ecdf</t>
         </is>
       </c>
     </row>
@@ -500,7 +500,7 @@
         <v>-0.147</v>
       </c>
       <c r="H2" t="n">
-        <v>0.01041666666666667</v>
+        <v>0.01052631578947368</v>
       </c>
     </row>
     <row r="3">
@@ -528,7 +528,7 @@
         <v>-0.077</v>
       </c>
       <c r="H3" t="n">
-        <v>0.02083333333333333</v>
+        <v>0.02105263157894737</v>
       </c>
     </row>
     <row r="4">
@@ -556,7 +556,7 @@
         <v>-0.043</v>
       </c>
       <c r="H4" t="n">
-        <v>0.03125</v>
+        <v>0.03157894736842105</v>
       </c>
     </row>
     <row r="5">
@@ -584,7 +584,7 @@
         <v>-0.037</v>
       </c>
       <c r="H5" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.04210526315789474</v>
       </c>
     </row>
     <row r="6">
@@ -612,7 +612,7 @@
         <v>-0.025</v>
       </c>
       <c r="H6" t="n">
-        <v>0.05208333333333333</v>
+        <v>0.05263157894736842</v>
       </c>
     </row>
     <row r="7">
@@ -640,7 +640,7 @@
         <v>-0.025</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0625</v>
+        <v>0.06315789473684211</v>
       </c>
     </row>
     <row r="8">
@@ -668,7 +668,7 @@
         <v>-0.022</v>
       </c>
       <c r="H8" t="n">
-        <v>0.07291666666666666</v>
+        <v>0.07368421052631578</v>
       </c>
     </row>
     <row r="9">
@@ -696,7 +696,7 @@
         <v>-0.022</v>
       </c>
       <c r="H9" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.08421052631578947</v>
       </c>
     </row>
     <row r="10">
@@ -724,7 +724,7 @@
         <v>-0.022</v>
       </c>
       <c r="H10" t="n">
-        <v>0.09375</v>
+        <v>0.09473684210526316</v>
       </c>
     </row>
     <row r="11">
@@ -752,7 +752,7 @@
         <v>-0.02</v>
       </c>
       <c r="H11" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.1052631578947368</v>
       </c>
     </row>
     <row r="12">
@@ -780,7 +780,7 @@
         <v>-0.018</v>
       </c>
       <c r="H12" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.1157894736842105</v>
       </c>
     </row>
     <row r="13">
@@ -808,7 +808,7 @@
         <v>-0.018</v>
       </c>
       <c r="H13" t="n">
-        <v>0.125</v>
+        <v>0.1263157894736842</v>
       </c>
     </row>
     <row r="14">
@@ -836,7 +836,7 @@
         <v>-0.018</v>
       </c>
       <c r="H14" t="n">
-        <v>0.1354166666666667</v>
+        <v>0.1368421052631579</v>
       </c>
     </row>
     <row r="15">
@@ -864,7 +864,7 @@
         <v>-0.015</v>
       </c>
       <c r="H15" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.1473684210526316</v>
       </c>
     </row>
     <row r="16">
@@ -892,7 +892,7 @@
         <v>-0.015</v>
       </c>
       <c r="H16" t="n">
-        <v>0.15625</v>
+        <v>0.1578947368421053</v>
       </c>
     </row>
     <row r="17">
@@ -920,7 +920,7 @@
         <v>-0.015</v>
       </c>
       <c r="H17" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.1684210526315789</v>
       </c>
     </row>
     <row r="18">
@@ -948,7 +948,7 @@
         <v>-0.015</v>
       </c>
       <c r="H18" t="n">
-        <v>0.1770833333333333</v>
+        <v>0.1789473684210526</v>
       </c>
     </row>
     <row r="19">
@@ -976,7 +976,7 @@
         <v>-0.015</v>
       </c>
       <c r="H19" t="n">
-        <v>0.1875</v>
+        <v>0.1894736842105263</v>
       </c>
     </row>
     <row r="20">
@@ -1004,7 +1004,7 @@
         <v>-0.013</v>
       </c>
       <c r="H20" t="n">
-        <v>0.1979166666666667</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="21">
@@ -1032,7 +1032,7 @@
         <v>-0.01</v>
       </c>
       <c r="H21" t="n">
-        <v>0.2083333333333333</v>
+        <v>0.2105263157894737</v>
       </c>
     </row>
     <row r="22">
@@ -1060,7 +1060,7 @@
         <v>-0.01</v>
       </c>
       <c r="H22" t="n">
-        <v>0.21875</v>
+        <v>0.2210526315789474</v>
       </c>
     </row>
     <row r="23">
@@ -1088,7 +1088,7 @@
         <v>-0.01</v>
       </c>
       <c r="H23" t="n">
-        <v>0.2291666666666667</v>
+        <v>0.2315789473684211</v>
       </c>
     </row>
     <row r="24">
@@ -1116,7 +1116,7 @@
         <v>-0.01</v>
       </c>
       <c r="H24" t="n">
-        <v>0.2395833333333333</v>
+        <v>0.2421052631578947</v>
       </c>
     </row>
     <row r="25">
@@ -1144,7 +1144,7 @@
         <v>-0.01</v>
       </c>
       <c r="H25" t="n">
-        <v>0.25</v>
+        <v>0.2526315789473684</v>
       </c>
     </row>
     <row r="26">
@@ -1172,7 +1172,7 @@
         <v>-0.007</v>
       </c>
       <c r="H26" t="n">
-        <v>0.2604166666666666</v>
+        <v>0.2631578947368421</v>
       </c>
     </row>
     <row r="27">
@@ -1200,7 +1200,7 @@
         <v>-0.007</v>
       </c>
       <c r="H27" t="n">
-        <v>0.2708333333333333</v>
+        <v>0.2736842105263158</v>
       </c>
     </row>
     <row r="28">
@@ -1228,7 +1228,7 @@
         <v>-0.007</v>
       </c>
       <c r="H28" t="n">
-        <v>0.28125</v>
+        <v>0.2842105263157895</v>
       </c>
     </row>
     <row r="29">
@@ -1256,7 +1256,7 @@
         <v>-0.007</v>
       </c>
       <c r="H29" t="n">
-        <v>0.2916666666666666</v>
+        <v>0.2947368421052631</v>
       </c>
     </row>
     <row r="30">
@@ -1284,7 +1284,7 @@
         <v>-0.007</v>
       </c>
       <c r="H30" t="n">
-        <v>0.3020833333333333</v>
+        <v>0.3052631578947368</v>
       </c>
     </row>
     <row r="31">
@@ -1312,7 +1312,7 @@
         <v>-0.007</v>
       </c>
       <c r="H31" t="n">
-        <v>0.3125</v>
+        <v>0.3157894736842105</v>
       </c>
     </row>
     <row r="32">
@@ -1340,7 +1340,7 @@
         <v>-0.007</v>
       </c>
       <c r="H32" t="n">
-        <v>0.3229166666666666</v>
+        <v>0.3263157894736842</v>
       </c>
     </row>
     <row r="33">
@@ -1368,7 +1368,7 @@
         <v>-0.007</v>
       </c>
       <c r="H33" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.3368421052631579</v>
       </c>
     </row>
     <row r="34">
@@ -1396,7 +1396,7 @@
         <v>-0.007</v>
       </c>
       <c r="H34" t="n">
-        <v>0.34375</v>
+        <v>0.3473684210526315</v>
       </c>
     </row>
     <row r="35">
@@ -1424,7 +1424,7 @@
         <v>-0.005</v>
       </c>
       <c r="H35" t="n">
-        <v>0.3541666666666666</v>
+        <v>0.3578947368421053</v>
       </c>
     </row>
     <row r="36">
@@ -1452,7 +1452,7 @@
         <v>-0.005</v>
       </c>
       <c r="H36" t="n">
-        <v>0.3645833333333333</v>
+        <v>0.3684210526315789</v>
       </c>
     </row>
     <row r="37">
@@ -1480,7 +1480,7 @@
         <v>-0.005</v>
       </c>
       <c r="H37" t="n">
-        <v>0.375</v>
+        <v>0.3789473684210526</v>
       </c>
     </row>
     <row r="38">
@@ -1508,7 +1508,7 @@
         <v>-0.005</v>
       </c>
       <c r="H38" t="n">
-        <v>0.3854166666666666</v>
+        <v>0.3894736842105263</v>
       </c>
     </row>
     <row r="39">
@@ -1536,7 +1536,7 @@
         <v>-0.005</v>
       </c>
       <c r="H39" t="n">
-        <v>0.3958333333333333</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="40">
@@ -1564,7 +1564,7 @@
         <v>-0.005</v>
       </c>
       <c r="H40" t="n">
-        <v>0.40625</v>
+        <v>0.4105263157894737</v>
       </c>
     </row>
     <row r="41">
@@ -1592,7 +1592,7 @@
         <v>-0.005</v>
       </c>
       <c r="H41" t="n">
-        <v>0.4166666666666666</v>
+        <v>0.4210526315789473</v>
       </c>
     </row>
     <row r="42">
@@ -1620,7 +1620,7 @@
         <v>-0.005</v>
       </c>
       <c r="H42" t="n">
-        <v>0.4270833333333333</v>
+        <v>0.4315789473684211</v>
       </c>
     </row>
     <row r="43">
@@ -1648,7 +1648,7 @@
         <v>-0.005</v>
       </c>
       <c r="H43" t="n">
-        <v>0.4375</v>
+        <v>0.4421052631578947</v>
       </c>
     </row>
     <row r="44">
@@ -1676,7 +1676,7 @@
         <v>-0.005</v>
       </c>
       <c r="H44" t="n">
-        <v>0.4479166666666666</v>
+        <v>0.4526315789473684</v>
       </c>
     </row>
     <row r="45">
@@ -1704,7 +1704,7 @@
         <v>-0.005</v>
       </c>
       <c r="H45" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.4631578947368421</v>
       </c>
     </row>
     <row r="46">
@@ -1732,7 +1732,7 @@
         <v>-0.003</v>
       </c>
       <c r="H46" t="n">
-        <v>0.46875</v>
+        <v>0.4736842105263158</v>
       </c>
     </row>
     <row r="47">
@@ -1760,7 +1760,7 @@
         <v>-0.003</v>
       </c>
       <c r="H47" t="n">
-        <v>0.4791666666666666</v>
+        <v>0.4842105263157895</v>
       </c>
     </row>
     <row r="48">
@@ -1788,7 +1788,7 @@
         <v>-0.003</v>
       </c>
       <c r="H48" t="n">
-        <v>0.4895833333333333</v>
+        <v>0.4947368421052631</v>
       </c>
     </row>
     <row r="49">
@@ -1816,7 +1816,7 @@
         <v>-0.003</v>
       </c>
       <c r="H49" t="n">
-        <v>0.5</v>
+        <v>0.5052631578947369</v>
       </c>
     </row>
     <row r="50">
@@ -1844,7 +1844,7 @@
         <v>-0.003</v>
       </c>
       <c r="H50" t="n">
-        <v>0.5104166666666666</v>
+        <v>0.5157894736842105</v>
       </c>
     </row>
     <row r="51">
@@ -1872,7 +1872,7 @@
         <v>-0.003</v>
       </c>
       <c r="H51" t="n">
-        <v>0.5208333333333333</v>
+        <v>0.5263157894736842</v>
       </c>
     </row>
     <row r="52">
@@ -1900,7 +1900,7 @@
         <v>-0.003</v>
       </c>
       <c r="H52" t="n">
-        <v>0.53125</v>
+        <v>0.5368421052631579</v>
       </c>
     </row>
     <row r="53">
@@ -1928,7 +1928,7 @@
         <v>-0.003</v>
       </c>
       <c r="H53" t="n">
-        <v>0.5416666666666666</v>
+        <v>0.5473684210526316</v>
       </c>
     </row>
     <row r="54">
@@ -1956,7 +1956,7 @@
         <v>-0.003</v>
       </c>
       <c r="H54" t="n">
-        <v>0.5520833333333333</v>
+        <v>0.5578947368421052</v>
       </c>
     </row>
     <row r="55">
@@ -1984,7 +1984,7 @@
         <v>0</v>
       </c>
       <c r="H55" t="n">
-        <v>0.5625</v>
+        <v>0.5684210526315789</v>
       </c>
     </row>
     <row r="56">
@@ -2012,7 +2012,7 @@
         <v>0</v>
       </c>
       <c r="H56" t="n">
-        <v>0.5729166666666666</v>
+        <v>0.5789473684210527</v>
       </c>
     </row>
     <row r="57">
@@ -2040,7 +2040,7 @@
         <v>0</v>
       </c>
       <c r="H57" t="n">
-        <v>0.5833333333333333</v>
+        <v>0.5894736842105263</v>
       </c>
     </row>
     <row r="58">
@@ -2068,7 +2068,7 @@
         <v>0</v>
       </c>
       <c r="H58" t="n">
-        <v>0.59375</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="59">
@@ -2096,7 +2096,7 @@
         <v>0</v>
       </c>
       <c r="H59" t="n">
-        <v>0.6041666666666666</v>
+        <v>0.6105263157894737</v>
       </c>
     </row>
     <row r="60">
@@ -2124,7 +2124,7 @@
         <v>0</v>
       </c>
       <c r="H60" t="n">
-        <v>0.6145833333333333</v>
+        <v>0.6210526315789473</v>
       </c>
     </row>
     <row r="61">
@@ -2152,7 +2152,7 @@
         <v>0.003</v>
       </c>
       <c r="H61" t="n">
-        <v>0.625</v>
+        <v>0.631578947368421</v>
       </c>
     </row>
     <row r="62">
@@ -2180,7 +2180,7 @@
         <v>0.003</v>
       </c>
       <c r="H62" t="n">
-        <v>0.6354166666666666</v>
+        <v>0.6421052631578947</v>
       </c>
     </row>
     <row r="63">
@@ -2208,7 +2208,7 @@
         <v>0.005</v>
       </c>
       <c r="H63" t="n">
-        <v>0.6458333333333333</v>
+        <v>0.6526315789473685</v>
       </c>
     </row>
     <row r="64">
@@ -2236,7 +2236,7 @@
         <v>0.005</v>
       </c>
       <c r="H64" t="n">
-        <v>0.65625</v>
+        <v>0.6631578947368421</v>
       </c>
     </row>
     <row r="65">
@@ -2264,7 +2264,7 @@
         <v>0.007</v>
       </c>
       <c r="H65" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6736842105263158</v>
       </c>
     </row>
     <row r="66">
@@ -2292,7 +2292,7 @@
         <v>0.007</v>
       </c>
       <c r="H66" t="n">
-        <v>0.6770833333333333</v>
+        <v>0.6842105263157895</v>
       </c>
     </row>
     <row r="67">
@@ -2320,7 +2320,7 @@
         <v>0.01</v>
       </c>
       <c r="H67" t="n">
-        <v>0.6875</v>
+        <v>0.6947368421052631</v>
       </c>
     </row>
     <row r="68">
@@ -2348,7 +2348,7 @@
         <v>0.01</v>
       </c>
       <c r="H68" t="n">
-        <v>0.6979166666666666</v>
+        <v>0.7052631578947368</v>
       </c>
     </row>
     <row r="69">
@@ -2376,7 +2376,7 @@
         <v>0.01</v>
       </c>
       <c r="H69" t="n">
-        <v>0.7083333333333333</v>
+        <v>0.7157894736842105</v>
       </c>
     </row>
     <row r="70">
@@ -2404,7 +2404,7 @@
         <v>0.01</v>
       </c>
       <c r="H70" t="n">
-        <v>0.71875</v>
+        <v>0.7263157894736842</v>
       </c>
     </row>
     <row r="71">
@@ -2432,7 +2432,7 @@
         <v>0.013</v>
       </c>
       <c r="H71" t="n">
-        <v>0.7291666666666666</v>
+        <v>0.7368421052631579</v>
       </c>
     </row>
     <row r="72">
@@ -2460,7 +2460,7 @@
         <v>0.013</v>
       </c>
       <c r="H72" t="n">
-        <v>0.7395833333333333</v>
+        <v>0.7473684210526316</v>
       </c>
     </row>
     <row r="73">
@@ -2488,7 +2488,7 @@
         <v>0.013</v>
       </c>
       <c r="H73" t="n">
-        <v>0.75</v>
+        <v>0.7578947368421053</v>
       </c>
     </row>
     <row r="74">
@@ -2516,7 +2516,7 @@
         <v>0.015</v>
       </c>
       <c r="H74" t="n">
-        <v>0.7604166666666666</v>
+        <v>0.7684210526315789</v>
       </c>
     </row>
     <row r="75">
@@ -2544,7 +2544,7 @@
         <v>0.015</v>
       </c>
       <c r="H75" t="n">
-        <v>0.7708333333333333</v>
+        <v>0.7789473684210526</v>
       </c>
     </row>
     <row r="76">
@@ -2572,7 +2572,7 @@
         <v>0.015</v>
       </c>
       <c r="H76" t="n">
-        <v>0.78125</v>
+        <v>0.7894736842105263</v>
       </c>
     </row>
     <row r="77">
@@ -2600,7 +2600,7 @@
         <v>0.015</v>
       </c>
       <c r="H77" t="n">
-        <v>0.7916666666666666</v>
+        <v>0.7999999999999999</v>
       </c>
     </row>
     <row r="78">
@@ -2628,7 +2628,7 @@
         <v>0.015</v>
       </c>
       <c r="H78" t="n">
-        <v>0.8020833333333333</v>
+        <v>0.8105263157894737</v>
       </c>
     </row>
     <row r="79">
@@ -2656,7 +2656,7 @@
         <v>0.015</v>
       </c>
       <c r="H79" t="n">
-        <v>0.8125</v>
+        <v>0.8210526315789474</v>
       </c>
     </row>
     <row r="80">
@@ -2684,7 +2684,7 @@
         <v>0.015</v>
       </c>
       <c r="H80" t="n">
-        <v>0.8229166666666666</v>
+        <v>0.8315789473684211</v>
       </c>
     </row>
     <row r="81">
@@ -2712,7 +2712,7 @@
         <v>0.015</v>
       </c>
       <c r="H81" t="n">
-        <v>0.8333333333333333</v>
+        <v>0.8421052631578947</v>
       </c>
     </row>
     <row r="82">
@@ -2740,7 +2740,7 @@
         <v>0.015</v>
       </c>
       <c r="H82" t="n">
-        <v>0.84375</v>
+        <v>0.8526315789473684</v>
       </c>
     </row>
     <row r="83">
@@ -2768,7 +2768,7 @@
         <v>0.018</v>
       </c>
       <c r="H83" t="n">
-        <v>0.8541666666666666</v>
+        <v>0.8631578947368421</v>
       </c>
     </row>
     <row r="84">
@@ -2796,7 +2796,7 @@
         <v>0.018</v>
       </c>
       <c r="H84" t="n">
-        <v>0.8645833333333333</v>
+        <v>0.8736842105263157</v>
       </c>
     </row>
     <row r="85">
@@ -2824,7 +2824,7 @@
         <v>0.018</v>
       </c>
       <c r="H85" t="n">
-        <v>0.875</v>
+        <v>0.8842105263157894</v>
       </c>
     </row>
     <row r="86">
@@ -2852,7 +2852,7 @@
         <v>0.02</v>
       </c>
       <c r="H86" t="n">
-        <v>0.8854166666666666</v>
+        <v>0.8947368421052632</v>
       </c>
     </row>
     <row r="87">
@@ -2880,7 +2880,7 @@
         <v>0.02</v>
       </c>
       <c r="H87" t="n">
-        <v>0.8958333333333333</v>
+        <v>0.9052631578947368</v>
       </c>
     </row>
     <row r="88">
@@ -2908,7 +2908,7 @@
         <v>0.02</v>
       </c>
       <c r="H88" t="n">
-        <v>0.90625</v>
+        <v>0.9157894736842105</v>
       </c>
     </row>
     <row r="89">
@@ -2936,7 +2936,7 @@
         <v>0.022</v>
       </c>
       <c r="H89" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.9263157894736842</v>
       </c>
     </row>
     <row r="90">
@@ -2964,7 +2964,7 @@
         <v>0.025</v>
       </c>
       <c r="H90" t="n">
-        <v>0.9270833333333333</v>
+        <v>0.9368421052631579</v>
       </c>
     </row>
     <row r="91">
@@ -2992,7 +2992,7 @@
         <v>0.025</v>
       </c>
       <c r="H91" t="n">
-        <v>0.9375</v>
+        <v>0.9473684210526315</v>
       </c>
     </row>
     <row r="92">
@@ -3020,7 +3020,7 @@
         <v>0.028</v>
       </c>
       <c r="H92" t="n">
-        <v>0.9479166666666666</v>
+        <v>0.9578947368421052</v>
       </c>
     </row>
     <row r="93">
@@ -3048,7 +3048,7 @@
         <v>0.03</v>
       </c>
       <c r="H93" t="n">
-        <v>0.9583333333333333</v>
+        <v>0.968421052631579</v>
       </c>
     </row>
     <row r="94">
@@ -3076,7 +3076,7 @@
         <v>0.03</v>
       </c>
       <c r="H94" t="n">
-        <v>0.96875</v>
+        <v>0.9789473684210526</v>
       </c>
     </row>
     <row r="95">
@@ -3104,7 +3104,7 @@
         <v>0.033</v>
       </c>
       <c r="H95" t="n">
-        <v>0.9791666666666666</v>
+        <v>0.9894736842105263</v>
       </c>
     </row>
     <row r="96">
@@ -3132,7 +3132,7 @@
         <v>0.043</v>
       </c>
       <c r="H96" t="n">
-        <v>0.9895833333333333</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the normal sample
</commit_message>
<xml_diff>
--- a/xlsx/stats.xlsx
+++ b/xlsx/stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H96"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,11 @@
           <t>ecdf</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>norm_sample</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -502,6 +507,9 @@
       <c r="H2" t="n">
         <v>0.01052631578947368</v>
       </c>
+      <c r="I2" t="n">
+        <v>-0.06884756893673077</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -530,6 +538,9 @@
       <c r="H3" t="n">
         <v>0.02105263157894737</v>
       </c>
+      <c r="I3" t="n">
+        <v>-0.05747885415475073</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -558,6 +569,9 @@
       <c r="H4" t="n">
         <v>0.03157894736842105</v>
       </c>
+      <c r="I4" t="n">
+        <v>-0.05409011469717837</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -586,6 +600,9 @@
       <c r="H5" t="n">
         <v>0.04210526315789474</v>
       </c>
+      <c r="I5" t="n">
+        <v>-0.04893597275464123</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -614,6 +631,9 @@
       <c r="H6" t="n">
         <v>0.05263157894736842</v>
       </c>
+      <c r="I6" t="n">
+        <v>-0.04270437276595071</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -642,6 +662,9 @@
       <c r="H7" t="n">
         <v>0.06315789473684211</v>
       </c>
+      <c r="I7" t="n">
+        <v>-0.04264752826659474</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -670,6 +693,9 @@
       <c r="H8" t="n">
         <v>0.07368421052631578</v>
       </c>
+      <c r="I8" t="n">
+        <v>-0.04045763297614108</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -698,6 +724,9 @@
       <c r="H9" t="n">
         <v>0.08421052631578947</v>
       </c>
+      <c r="I9" t="n">
+        <v>-0.03435591152980129</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -726,6 +755,9 @@
       <c r="H10" t="n">
         <v>0.09473684210526316</v>
       </c>
+      <c r="I10" t="n">
+        <v>-0.03290726718297413</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -754,6 +786,9 @@
       <c r="H11" t="n">
         <v>0.1052631578947368</v>
       </c>
+      <c r="I11" t="n">
+        <v>-0.03104092188805441</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -782,6 +817,9 @@
       <c r="H12" t="n">
         <v>0.1157894736842105</v>
       </c>
+      <c r="I12" t="n">
+        <v>-0.028556055836795</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -810,6 +848,9 @@
       <c r="H13" t="n">
         <v>0.1263157894736842</v>
       </c>
+      <c r="I13" t="n">
+        <v>-0.02679669085194228</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -838,6 +879,9 @@
       <c r="H14" t="n">
         <v>0.1368421052631579</v>
       </c>
+      <c r="I14" t="n">
+        <v>-0.02643806212275866</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -866,6 +910,9 @@
       <c r="H15" t="n">
         <v>0.1473684210526316</v>
       </c>
+      <c r="I15" t="n">
+        <v>-0.02552513068504525</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -894,6 +941,9 @@
       <c r="H16" t="n">
         <v>0.1578947368421053</v>
       </c>
+      <c r="I16" t="n">
+        <v>-0.02316557483509203</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -922,6 +972,9 @@
       <c r="H17" t="n">
         <v>0.1684210526315789</v>
       </c>
+      <c r="I17" t="n">
+        <v>-0.02313972646396837</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -950,6 +1003,9 @@
       <c r="H18" t="n">
         <v>0.1789473684210526</v>
       </c>
+      <c r="I18" t="n">
+        <v>-0.0212821417883994</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -978,6 +1034,9 @@
       <c r="H19" t="n">
         <v>0.1894736842105263</v>
       </c>
+      <c r="I19" t="n">
+        <v>-0.02017259528916622</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1006,6 +1065,9 @@
       <c r="H20" t="n">
         <v>0.2</v>
       </c>
+      <c r="I20" t="n">
+        <v>-0.01974285654372802</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1034,6 +1096,9 @@
       <c r="H21" t="n">
         <v>0.2105263157894737</v>
       </c>
+      <c r="I21" t="n">
+        <v>-0.0187100333554594</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1062,6 +1127,9 @@
       <c r="H22" t="n">
         <v>0.2210526315789474</v>
       </c>
+      <c r="I22" t="n">
+        <v>-0.01794010598874173</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1090,6 +1158,9 @@
       <c r="H23" t="n">
         <v>0.2315789473684211</v>
       </c>
+      <c r="I23" t="n">
+        <v>-0.01733577913495614</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1118,6 +1189,9 @@
       <c r="H24" t="n">
         <v>0.2421052631578947</v>
       </c>
+      <c r="I24" t="n">
+        <v>-0.01642362578693973</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1146,6 +1220,9 @@
       <c r="H25" t="n">
         <v>0.2526315789473684</v>
       </c>
+      <c r="I25" t="n">
+        <v>-0.0159266714797445</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1174,6 +1251,9 @@
       <c r="H26" t="n">
         <v>0.2631578947368421</v>
       </c>
+      <c r="I26" t="n">
+        <v>-0.01485750084075787</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1202,6 +1282,9 @@
       <c r="H27" t="n">
         <v>0.2736842105263158</v>
       </c>
+      <c r="I27" t="n">
+        <v>-0.01472186685021784</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1230,6 +1313,9 @@
       <c r="H28" t="n">
         <v>0.2842105263157895</v>
       </c>
+      <c r="I28" t="n">
+        <v>-0.01398161163124536</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1258,6 +1344,9 @@
       <c r="H29" t="n">
         <v>0.2947368421052631</v>
       </c>
+      <c r="I29" t="n">
+        <v>-0.01358951627189297</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1286,6 +1375,9 @@
       <c r="H30" t="n">
         <v>0.3052631578947368</v>
       </c>
+      <c r="I30" t="n">
+        <v>-0.01331279720686511</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1314,6 +1406,9 @@
       <c r="H31" t="n">
         <v>0.3157894736842105</v>
       </c>
+      <c r="I31" t="n">
+        <v>-0.01295535249349514</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1342,6 +1437,9 @@
       <c r="H32" t="n">
         <v>0.3263157894736842</v>
       </c>
+      <c r="I32" t="n">
+        <v>-0.01116226779421779</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1370,6 +1468,9 @@
       <c r="H33" t="n">
         <v>0.3368421052631579</v>
       </c>
+      <c r="I33" t="n">
+        <v>-0.01111284894134258</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1398,6 +1499,9 @@
       <c r="H34" t="n">
         <v>0.3473684210526315</v>
       </c>
+      <c r="I34" t="n">
+        <v>-0.01022384370548639</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1426,6 +1530,9 @@
       <c r="H35" t="n">
         <v>0.3578947368421053</v>
       </c>
+      <c r="I35" t="n">
+        <v>-0.01015481704480267</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1454,6 +1561,9 @@
       <c r="H36" t="n">
         <v>0.3684210526315789</v>
       </c>
+      <c r="I36" t="n">
+        <v>-0.01008915410924837</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1482,6 +1592,9 @@
       <c r="H37" t="n">
         <v>0.3789473684210526</v>
       </c>
+      <c r="I37" t="n">
+        <v>-0.009257830926931814</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1510,6 +1623,9 @@
       <c r="H38" t="n">
         <v>0.3894736842105263</v>
       </c>
+      <c r="I38" t="n">
+        <v>-0.008239367445834081</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1538,6 +1654,9 @@
       <c r="H39" t="n">
         <v>0.4</v>
       </c>
+      <c r="I39" t="n">
+        <v>-0.008234710748315281</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -1566,6 +1685,9 @@
       <c r="H40" t="n">
         <v>0.4105263157894737</v>
       </c>
+      <c r="I40" t="n">
+        <v>-0.006187766520348362</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -1594,6 +1716,9 @@
       <c r="H41" t="n">
         <v>0.4210526315789473</v>
       </c>
+      <c r="I41" t="n">
+        <v>-0.004802629570806549</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -1622,6 +1747,9 @@
       <c r="H42" t="n">
         <v>0.4315789473684211</v>
       </c>
+      <c r="I42" t="n">
+        <v>-0.004324588592705947</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1650,6 +1778,9 @@
       <c r="H43" t="n">
         <v>0.4421052631578947</v>
       </c>
+      <c r="I43" t="n">
+        <v>-0.003274872137717096</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1678,6 +1809,9 @@
       <c r="H44" t="n">
         <v>0.4526315789473684</v>
       </c>
+      <c r="I44" t="n">
+        <v>-0.002664264109184237</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -1706,6 +1840,9 @@
       <c r="H45" t="n">
         <v>0.4631578947368421</v>
       </c>
+      <c r="I45" t="n">
+        <v>-0.002644876547946708</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1734,6 +1871,9 @@
       <c r="H46" t="n">
         <v>0.4736842105263158</v>
       </c>
+      <c r="I46" t="n">
+        <v>-0.00257317950560736</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1762,6 +1902,9 @@
       <c r="H47" t="n">
         <v>0.4842105263157895</v>
       </c>
+      <c r="I47" t="n">
+        <v>-0.001938412156323156</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -1790,6 +1933,9 @@
       <c r="H48" t="n">
         <v>0.4947368421052631</v>
       </c>
+      <c r="I48" t="n">
+        <v>-0.0009821958358117336</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1818,6 +1964,9 @@
       <c r="H49" t="n">
         <v>0.5052631578947369</v>
       </c>
+      <c r="I49" t="n">
+        <v>-0.0004444190928998785</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1846,6 +1995,9 @@
       <c r="H50" t="n">
         <v>0.5157894736842105</v>
       </c>
+      <c r="I50" t="n">
+        <v>0.0003149312196317896</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -1874,6 +2026,9 @@
       <c r="H51" t="n">
         <v>0.5263157894736842</v>
       </c>
+      <c r="I51" t="n">
+        <v>0.001734303913876858</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -1902,6 +2057,9 @@
       <c r="H52" t="n">
         <v>0.5368421052631579</v>
       </c>
+      <c r="I52" t="n">
+        <v>0.001905627237624808</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -1930,6 +2088,9 @@
       <c r="H53" t="n">
         <v>0.5473684210526316</v>
       </c>
+      <c r="I53" t="n">
+        <v>0.002060168879335924</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -1958,6 +2119,9 @@
       <c r="H54" t="n">
         <v>0.5578947368421052</v>
       </c>
+      <c r="I54" t="n">
+        <v>0.002785159436380215</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -1986,6 +2150,9 @@
       <c r="H55" t="n">
         <v>0.5684210526315789</v>
       </c>
+      <c r="I55" t="n">
+        <v>0.003175512489880537</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -2014,6 +2181,9 @@
       <c r="H56" t="n">
         <v>0.5789473684210527</v>
       </c>
+      <c r="I56" t="n">
+        <v>0.003453511046511433</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -2042,6 +2212,9 @@
       <c r="H57" t="n">
         <v>0.5894736842105263</v>
       </c>
+      <c r="I57" t="n">
+        <v>0.004233166909151772</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -2070,6 +2243,9 @@
       <c r="H58" t="n">
         <v>0.6</v>
       </c>
+      <c r="I58" t="n">
+        <v>0.00437837429349911</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -2098,6 +2274,9 @@
       <c r="H59" t="n">
         <v>0.6105263157894737</v>
       </c>
+      <c r="I59" t="n">
+        <v>0.006393850650235813</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -2126,6 +2305,9 @@
       <c r="H60" t="n">
         <v>0.6210526315789473</v>
       </c>
+      <c r="I60" t="n">
+        <v>0.007030265213488995</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -2154,6 +2336,9 @@
       <c r="H61" t="n">
         <v>0.631578947368421</v>
       </c>
+      <c r="I61" t="n">
+        <v>0.007347836654934577</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -2182,6 +2367,9 @@
       <c r="H62" t="n">
         <v>0.6421052631578947</v>
       </c>
+      <c r="I62" t="n">
+        <v>0.007643478670453655</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -2210,6 +2398,9 @@
       <c r="H63" t="n">
         <v>0.6526315789473685</v>
       </c>
+      <c r="I63" t="n">
+        <v>0.007726608419276571</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -2238,6 +2429,9 @@
       <c r="H64" t="n">
         <v>0.6631578947368421</v>
       </c>
+      <c r="I64" t="n">
+        <v>0.008084802244504889</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -2266,6 +2460,9 @@
       <c r="H65" t="n">
         <v>0.6736842105263158</v>
       </c>
+      <c r="I65" t="n">
+        <v>0.008521509237455907</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -2294,6 +2491,9 @@
       <c r="H66" t="n">
         <v>0.6842105263157895</v>
       </c>
+      <c r="I66" t="n">
+        <v>0.009073449296860367</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -2322,6 +2522,9 @@
       <c r="H67" t="n">
         <v>0.6947368421052631</v>
       </c>
+      <c r="I67" t="n">
+        <v>0.009992845817947507</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -2350,6 +2553,9 @@
       <c r="H68" t="n">
         <v>0.7052631578947368</v>
       </c>
+      <c r="I68" t="n">
+        <v>0.01026845215075704</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -2378,6 +2584,9 @@
       <c r="H69" t="n">
         <v>0.7157894736842105</v>
       </c>
+      <c r="I69" t="n">
+        <v>0.01099613608185137</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -2406,6 +2615,9 @@
       <c r="H70" t="n">
         <v>0.7263157894736842</v>
       </c>
+      <c r="I70" t="n">
+        <v>0.0141101164532052</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -2434,6 +2646,9 @@
       <c r="H71" t="n">
         <v>0.7368421052631579</v>
       </c>
+      <c r="I71" t="n">
+        <v>0.01520595310196653</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -2462,6 +2677,9 @@
       <c r="H72" t="n">
         <v>0.7473684210526316</v>
       </c>
+      <c r="I72" t="n">
+        <v>0.01545001307148072</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -2490,6 +2708,9 @@
       <c r="H73" t="n">
         <v>0.7578947368421053</v>
       </c>
+      <c r="I73" t="n">
+        <v>0.01579339777863938</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -2518,6 +2739,9 @@
       <c r="H74" t="n">
         <v>0.7684210526315789</v>
       </c>
+      <c r="I74" t="n">
+        <v>0.01605276762101358</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -2546,6 +2770,9 @@
       <c r="H75" t="n">
         <v>0.7789473684210526</v>
       </c>
+      <c r="I75" t="n">
+        <v>0.01631449483921896</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -2574,6 +2801,9 @@
       <c r="H76" t="n">
         <v>0.7894736842105263</v>
       </c>
+      <c r="I76" t="n">
+        <v>0.01883576485206128</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -2602,6 +2832,9 @@
       <c r="H77" t="n">
         <v>0.7999999999999999</v>
       </c>
+      <c r="I77" t="n">
+        <v>0.01944224292139983</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -2630,6 +2863,9 @@
       <c r="H78" t="n">
         <v>0.8105263157894737</v>
       </c>
+      <c r="I78" t="n">
+        <v>0.01947556215657805</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -2658,6 +2894,9 @@
       <c r="H79" t="n">
         <v>0.8210526315789474</v>
       </c>
+      <c r="I79" t="n">
+        <v>0.02083281027531672</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -2686,6 +2925,9 @@
       <c r="H80" t="n">
         <v>0.8315789473684211</v>
       </c>
+      <c r="I80" t="n">
+        <v>0.02125990775286905</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -2714,6 +2956,9 @@
       <c r="H81" t="n">
         <v>0.8421052631578947</v>
       </c>
+      <c r="I81" t="n">
+        <v>0.02204494578394293</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -2742,6 +2987,9 @@
       <c r="H82" t="n">
         <v>0.8526315789473684</v>
       </c>
+      <c r="I82" t="n">
+        <v>0.02435477551692228</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -2770,6 +3018,9 @@
       <c r="H83" t="n">
         <v>0.8631578947368421</v>
       </c>
+      <c r="I83" t="n">
+        <v>0.0270170088350674</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -2798,6 +3049,9 @@
       <c r="H84" t="n">
         <v>0.8736842105263157</v>
       </c>
+      <c r="I84" t="n">
+        <v>0.02842940002001671</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -2826,6 +3080,9 @@
       <c r="H85" t="n">
         <v>0.8842105263157894</v>
       </c>
+      <c r="I85" t="n">
+        <v>0.02846059321963981</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -2854,6 +3111,9 @@
       <c r="H86" t="n">
         <v>0.8947368421052632</v>
       </c>
+      <c r="I86" t="n">
+        <v>0.02905969938468173</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -2882,6 +3142,9 @@
       <c r="H87" t="n">
         <v>0.9052631578947368</v>
       </c>
+      <c r="I87" t="n">
+        <v>0.03014550406742116</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -2910,6 +3173,9 @@
       <c r="H88" t="n">
         <v>0.9157894736842105</v>
       </c>
+      <c r="I88" t="n">
+        <v>0.03038788186466854</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -2938,6 +3204,9 @@
       <c r="H89" t="n">
         <v>0.9263157894736842</v>
       </c>
+      <c r="I89" t="n">
+        <v>0.03053181655111144</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -2966,6 +3235,9 @@
       <c r="H90" t="n">
         <v>0.9368421052631579</v>
       </c>
+      <c r="I90" t="n">
+        <v>0.03062073717900662</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -2994,6 +3266,9 @@
       <c r="H91" t="n">
         <v>0.9473684210526315</v>
       </c>
+      <c r="I91" t="n">
+        <v>0.03212137827295825</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -3022,6 +3297,9 @@
       <c r="H92" t="n">
         <v>0.9578947368421052</v>
       </c>
+      <c r="I92" t="n">
+        <v>0.03230174570592321</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -3050,6 +3328,9 @@
       <c r="H93" t="n">
         <v>0.968421052631579</v>
       </c>
+      <c r="I93" t="n">
+        <v>0.03241406151680494</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -3078,6 +3359,9 @@
       <c r="H94" t="n">
         <v>0.9789473684210526</v>
       </c>
+      <c r="I94" t="n">
+        <v>0.0443311401490801</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -3106,6 +3390,9 @@
       <c r="H95" t="n">
         <v>0.9894736842105263</v>
       </c>
+      <c r="I95" t="n">
+        <v>0.04517453033017867</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -3133,6 +3420,9 @@
       </c>
       <c r="H96" t="n">
         <v>1</v>
+      </c>
+      <c r="I96" t="n">
+        <v>0.04715823800072949</v>
       </c>
     </row>
   </sheetData>

</xml_diff>